<commit_message>
Added JAR for the first release.
</commit_message>
<xml_diff>
--- a/target/classes/out/fr.xlsx
+++ b/target/classes/out/fr.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="144">
   <si>
     <t>WORD</t>
   </si>
@@ -23,6 +23,21 @@
     <t>FREQUENCY</t>
   </si>
   <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
     <t>жизни</t>
   </si>
   <si>
@@ -32,6 +47,12 @@
     <t>7</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>радость</t>
   </si>
   <si>
@@ -41,12 +62,15 @@
     <t>цель</t>
   </si>
   <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>людям</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>19</t>
   </si>
   <si>
@@ -56,6 +80,9 @@
     <t>2</t>
   </si>
   <si>
+    <t>:</t>
+  </si>
+  <si>
     <t>атмосферу</t>
   </si>
   <si>
@@ -92,7 +119,7 @@
     <t>человека</t>
   </si>
   <si>
-    <t>18</t>
+    <t>!</t>
   </si>
   <si>
     <t>1</t>
@@ -105,6 +132,12 @@
   </si>
   <si>
     <t>english</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>some</t>
   </si>
   <si>
     <t>words</t>
@@ -455,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C122"/>
+  <dimension ref="A1:C130"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -499,1308 +532,1396 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
         <v>38</v>
       </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C54" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B59" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B60" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B61" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B67" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B70" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B71" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C71" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C73" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B75" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B76" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B77" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C77" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B78" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C78" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C79" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B80" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C80" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B81" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C81" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C82" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B83" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C83" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C84" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B85" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C85" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B86" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B87" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C87" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C88" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B89" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C89" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C90" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B91" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C91" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B92" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C92" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B93" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C93" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C94" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B95" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B96" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C96" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C97" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B98" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B99" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C99" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B100" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B101" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C101" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B102" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C102" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B103" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C103" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B104" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C104" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B105" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C105" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B106" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C106" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B107" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C107" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B108" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C108" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B109" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C109" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B110" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C110" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B111" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C111" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B112" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C112" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B113" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C113" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C114" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B115" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C115" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B116" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C116" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B117" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C117" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B118" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C118" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B119" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C119" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B120" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C120" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B121" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C121" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B122" t="s">
-        <v>132</v>
+        <v>9</v>
       </c>
       <c r="C122" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>135</v>
+      </c>
+      <c r="B123" t="s">
+        <v>9</v>
+      </c>
+      <c r="C123" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>136</v>
+      </c>
+      <c r="B124" t="s">
+        <v>9</v>
+      </c>
+      <c r="C124" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>137</v>
+      </c>
+      <c r="B125" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>138</v>
+      </c>
+      <c r="B126" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>139</v>
+      </c>
+      <c r="B127" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>140</v>
+      </c>
+      <c r="B128" t="s">
+        <v>9</v>
+      </c>
+      <c r="C128" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>141</v>
+      </c>
+      <c r="B129" t="s">
+        <v>9</v>
+      </c>
+      <c r="C129" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>142</v>
+      </c>
+      <c r="B130" t="s">
+        <v>143</v>
+      </c>
+      <c r="C130" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>